<commit_message>
The workflow up to the "Classification" part
</commit_message>
<xml_diff>
--- a/DocumentProcessing/Config.xlsx
+++ b/DocumentProcessing/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Videos\Document Understanding\DUFramework\DocumentProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAC568A-3617-46E3-9245-BB586EC773B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6326C10-17BB-4395-AF1A-A326B660EBC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -39,17 +39,38 @@
     <t>EndProcessMessage</t>
   </si>
   <si>
-    <t>ApiKey</t>
-  </si>
-  <si>
-    <t>Endpoint</t>
+    <t>OCREndpoint</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>The path of the directory in which the files to be processed are stored</t>
+  </si>
+  <si>
+    <t>The message that should be displayed when the workflow execution ends</t>
+  </si>
+  <si>
+    <t>The OCR Engine API Key</t>
+  </si>
+  <si>
+    <t>The OCR Engine endpoint</t>
+  </si>
+  <si>
+    <t>OCRApiKey</t>
+  </si>
+  <si>
+    <t>The Document Understanding API Key</t>
+  </si>
+  <si>
+    <t>DUApiKey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +82,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,14 +112,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,44 +401,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="C6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The workflow up to the "Data Exportation" point
</commit_message>
<xml_diff>
--- a/DocumentProcessing/Config.xlsx
+++ b/DocumentProcessing/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Videos\Document Understanding\DUFramework\DocumentProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6326C10-17BB-4395-AF1A-A326B660EBC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1844B9D-A894-4FCD-B102-27F6373C31CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +90,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,10 +122,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -404,7 +411,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +460,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -462,6 +469,7 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>9</v>
       </c>

</xml_diff>